<commit_message>
updated analysis for all participants. addressed unequal trial #s in tuning
</commit_message>
<xml_diff>
--- a/ExcelFiles/s4_good_trials_GraspObject_Combined.xlsx
+++ b/ExcelFiles/s4_good_trials_GraspObject_Combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD0D2CB-F3CD-442B-8693-59D7E5A4DBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E93A6CC-110A-4A28-B893-418292E044E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="2640" windowWidth="12150" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +575,65 @@
         <v>12</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20250818</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20250820</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>